<commit_message>
update data & programming.
</commit_message>
<xml_diff>
--- a/Documents/Problem 2 & 3 - Lamps.xlsx
+++ b/Documents/Problem 2 & 3 - Lamps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/easonshao/Documents/开发/For-November-IMMC-Competition/IMMC_2022_Greater_China/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6684C34-9A0A-804E-8D02-F794259046D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4DF5D0-2430-BF4B-A4A6-239E872D6970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="22100" windowWidth="28800" windowHeight="16840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Data" sheetId="1" r:id="rId1"/>
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F66000F-B72A-E94F-934D-D43F8EA6B34C}">
   <dimension ref="A1:S100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3496,7 +3496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C11F3088-1808-0E43-80A6-099B893D3AEF}">
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>

</xml_diff>